<commit_message>
added all interpretable models results
</commit_message>
<xml_diff>
--- a/ky-fl-combined/ky-model/results/baselines/two-year/two-year-ky-baseline.xlsx
+++ b/ky-fl-combined/ky-model/results/baselines/two-year/two-year-ky-baseline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22604"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\OICE_16_974FA576_32C1D314_172B\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\binha\Documents\Duke\Cynthia Research\interpretable-machine-learning\ky-fl-combined\ky-model\results\baselines\two-year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAFA20BD-7782-49F2-9508-5D25CD819FA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B29F65C-A2FB-4CA8-8AB0-73C47021063E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11760"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -982,14 +982,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1006,7 +1008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1026,103 +1028,103 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>21</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>26</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>27</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>31</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>33</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>35</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>37</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>39</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>